<commit_message>
update tabelas e inicio Testes
</commit_message>
<xml_diff>
--- a/Tabelas equivalência e casos de teste.xlsx
+++ b/Tabelas equivalência e casos de teste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vieir\Documents\GitHub\ESII--TP2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{101E0DF3-4A24-4000-92F2-8D4C275665A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9549000F-432B-4404-A90F-F01AA670D52E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="81">
   <si>
     <t>Critério</t>
   </si>
@@ -102,9 +102,6 @@
   </si>
   <si>
     <t>tratamentoPalavras</t>
-  </si>
-  <si>
-    <t>numFiles - int</t>
   </si>
   <si>
     <t>numFiles &gt; 0</t>
@@ -644,52 +641,52 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1073,8 +1070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="B114" sqref="B114"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1100,11 +1097,11 @@
       <c r="B2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="78" t="s">
+      <c r="C2" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -1113,11 +1110,11 @@
       <c r="B3" s="3">
         <v>1</v>
       </c>
-      <c r="C3" s="67" t="s">
+      <c r="C3" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="68"/>
-      <c r="E3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="70"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -1126,11 +1123,11 @@
       <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="70" t="s">
+      <c r="C4" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="71"/>
-      <c r="E4" s="72"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="73"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -1139,24 +1136,24 @@
       <c r="B5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="73" t="s">
+      <c r="C5" s="74" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="74"/>
-      <c r="E5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="76"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C6" s="76"/>
-      <c r="D6" s="76"/>
-      <c r="E6" s="76"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B7" s="78" t="s">
+      <c r="B7" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="79"/>
-      <c r="D7" s="79"/>
-      <c r="E7" s="79"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="78"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B8" s="35" t="s">
@@ -1199,14 +1196,14 @@
       <c r="E12" s="33"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C13" s="76"/>
-      <c r="D13" s="76"/>
-      <c r="E13" s="76"/>
+      <c r="C13" s="64"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="64"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C14" s="64"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="64"/>
+      <c r="C14" s="79"/>
+      <c r="D14" s="79"/>
+      <c r="E14" s="79"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="24"/>
@@ -1224,11 +1221,11 @@
       <c r="B16" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="78" t="s">
+      <c r="C16" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="79"/>
-      <c r="E16" s="79"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="78"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
@@ -1237,11 +1234,11 @@
       <c r="B17" s="3">
         <v>1</v>
       </c>
-      <c r="C17" s="67" t="s">
+      <c r="C17" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="68"/>
-      <c r="E17" s="69"/>
+      <c r="D17" s="69"/>
+      <c r="E17" s="70"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
@@ -1250,11 +1247,11 @@
       <c r="B18" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="70" t="s">
+      <c r="C18" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="71"/>
-      <c r="E18" s="72"/>
+      <c r="D18" s="72"/>
+      <c r="E18" s="73"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
@@ -1263,24 +1260,24 @@
       <c r="B19" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="73" t="s">
+      <c r="C19" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="74"/>
-      <c r="E19" s="75"/>
+      <c r="D19" s="75"/>
+      <c r="E19" s="76"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C20" s="76"/>
-      <c r="D20" s="76"/>
-      <c r="E20" s="76"/>
+      <c r="C20" s="64"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="64"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B21" s="78" t="s">
+      <c r="B21" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="79"/>
-      <c r="D21" s="79"/>
-      <c r="E21" s="79"/>
+      <c r="C21" s="78"/>
+      <c r="D21" s="78"/>
+      <c r="E21" s="78"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B22" s="35" t="s">
@@ -1351,42 +1348,42 @@
       <c r="B31" s="3">
         <v>1</v>
       </c>
-      <c r="C31" s="67" t="s">
+      <c r="C31" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="D31" s="68"/>
-      <c r="E31" s="69"/>
+      <c r="D31" s="69"/>
+      <c r="E31" s="70"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C32" s="70" t="s">
-        <v>26</v>
-      </c>
-      <c r="D32" s="71"/>
-      <c r="E32" s="72"/>
+        <v>79</v>
+      </c>
+      <c r="C32" s="71" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" s="72"/>
+      <c r="E32" s="73"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C33" s="73" t="s">
-        <v>27</v>
-      </c>
-      <c r="D33" s="74"/>
-      <c r="E33" s="75"/>
+        <v>24</v>
+      </c>
+      <c r="C33" s="74" t="s">
+        <v>26</v>
+      </c>
+      <c r="D33" s="75"/>
+      <c r="E33" s="76"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C34" s="76"/>
-      <c r="D34" s="76"/>
-      <c r="E34" s="76"/>
+      <c r="C34" s="64"/>
+      <c r="D34" s="64"/>
+      <c r="E34" s="64"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B35" s="18" t="s">
@@ -1398,7 +1395,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B36" s="35" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C36" s="6"/>
       <c r="D36" s="7"/>
@@ -1406,7 +1403,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B37" s="35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C37" s="9"/>
       <c r="D37" s="10"/>
@@ -1414,7 +1411,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B38" s="35" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C38" s="9"/>
       <c r="D38" s="10"/>
@@ -1422,7 +1419,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B39" s="35" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C39" s="12"/>
       <c r="D39" s="13"/>
@@ -1430,26 +1427,26 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B40" s="35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C40" s="15"/>
       <c r="D40" s="16"/>
       <c r="E40" s="17"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C41" s="76"/>
-      <c r="D41" s="76"/>
-      <c r="E41" s="76"/>
+      <c r="C41" s="64"/>
+      <c r="D41" s="64"/>
+      <c r="E41" s="64"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C42" s="77"/>
-      <c r="D42" s="77"/>
-      <c r="E42" s="77"/>
+      <c r="C42" s="67"/>
+      <c r="D42" s="67"/>
+      <c r="E42" s="67"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="24"/>
       <c r="B43" s="65" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C43" s="65"/>
       <c r="D43" s="65"/>
@@ -1475,42 +1472,42 @@
       <c r="B45" s="3">
         <v>1</v>
       </c>
-      <c r="C45" s="67" t="s">
+      <c r="C45" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="D45" s="68"/>
-      <c r="E45" s="69"/>
+      <c r="D45" s="69"/>
+      <c r="E45" s="70"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C46" s="70" t="s">
-        <v>26</v>
-      </c>
-      <c r="D46" s="71"/>
-      <c r="E46" s="72"/>
+        <v>79</v>
+      </c>
+      <c r="C46" s="71" t="s">
+        <v>25</v>
+      </c>
+      <c r="D46" s="72"/>
+      <c r="E46" s="73"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C47" s="73" t="s">
-        <v>27</v>
-      </c>
-      <c r="D47" s="74"/>
-      <c r="E47" s="75"/>
+        <v>24</v>
+      </c>
+      <c r="C47" s="74" t="s">
+        <v>26</v>
+      </c>
+      <c r="D47" s="75"/>
+      <c r="E47" s="76"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C48" s="76"/>
-      <c r="D48" s="76"/>
-      <c r="E48" s="76"/>
+      <c r="C48" s="64"/>
+      <c r="D48" s="64"/>
+      <c r="E48" s="64"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B49" s="62" t="s">
@@ -1522,7 +1519,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B50" s="35" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C50" s="6"/>
       <c r="D50" s="7"/>
@@ -1530,7 +1527,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B51" s="35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C51" s="55"/>
       <c r="D51" s="56"/>
@@ -1538,7 +1535,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B52" s="35" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C52" s="55"/>
       <c r="D52" s="56"/>
@@ -1546,7 +1543,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B53" s="35" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C53" s="49"/>
       <c r="D53" s="50"/>
@@ -1554,7 +1551,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B54" s="35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C54" s="52"/>
       <c r="D54" s="53"/>
@@ -1563,7 +1560,7 @@
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="24"/>
       <c r="B57" s="58" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C57" s="58"/>
       <c r="D57" s="58"/>
@@ -1600,10 +1597,10 @@
         <v>4</v>
       </c>
       <c r="B60" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C60" s="49" t="s">
         <v>35</v>
-      </c>
-      <c r="C60" s="49" t="s">
-        <v>36</v>
       </c>
       <c r="D60" s="50"/>
       <c r="E60" s="51"/>
@@ -1613,10 +1610,10 @@
         <v>5</v>
       </c>
       <c r="B61" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C61" s="52" t="s">
         <v>37</v>
-      </c>
-      <c r="C61" s="52" t="s">
-        <v>38</v>
       </c>
       <c r="D61" s="53"/>
       <c r="E61" s="54"/>
@@ -1636,7 +1633,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B64" s="35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C64" s="6"/>
       <c r="D64" s="7"/>
@@ -1644,7 +1641,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B65" s="35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C65" s="55"/>
       <c r="D65" s="56"/>
@@ -1652,7 +1649,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B66" s="35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C66" s="55"/>
       <c r="D66" s="56"/>
@@ -1660,7 +1657,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B67" s="35" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C67" s="49"/>
       <c r="D67" s="50"/>
@@ -1668,7 +1665,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B68" s="35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C68" s="49"/>
       <c r="D68" s="50"/>
@@ -1676,7 +1673,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B69" s="35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C69" s="49"/>
       <c r="D69" s="50"/>
@@ -1684,7 +1681,7 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B70" s="35" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C70" s="52"/>
       <c r="D70" s="53"/>
@@ -1692,7 +1689,7 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B71" s="35" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C71" s="52"/>
       <c r="D71" s="53"/>
@@ -1700,7 +1697,7 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B72" s="35" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C72" s="52"/>
       <c r="D72" s="53"/>
@@ -1719,7 +1716,7 @@
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="24"/>
       <c r="B75" s="58" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C75" s="58"/>
       <c r="D75" s="58"/>
@@ -1756,10 +1753,10 @@
         <v>4</v>
       </c>
       <c r="B78" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C78" s="49" t="s">
         <v>49</v>
-      </c>
-      <c r="C78" s="49" t="s">
-        <v>50</v>
       </c>
       <c r="D78" s="50"/>
       <c r="E78" s="51"/>
@@ -1769,10 +1766,10 @@
         <v>5</v>
       </c>
       <c r="B79" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C79" s="52" t="s">
         <v>51</v>
-      </c>
-      <c r="C79" s="52" t="s">
-        <v>52</v>
       </c>
       <c r="D79" s="53"/>
       <c r="E79" s="54"/>
@@ -1792,7 +1789,7 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B82" s="35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C82" s="6"/>
       <c r="D82" s="7"/>
@@ -1800,7 +1797,7 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B83" s="35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C83" s="55"/>
       <c r="D83" s="56"/>
@@ -1808,7 +1805,7 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B84" s="35" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C84" s="55"/>
       <c r="D84" s="56"/>
@@ -1816,7 +1813,7 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B85" s="35" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C85" s="49"/>
       <c r="D85" s="50"/>
@@ -1824,7 +1821,7 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B86" s="35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C86" s="49"/>
       <c r="D86" s="50"/>
@@ -1832,7 +1829,7 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B87" s="35" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C87" s="49"/>
       <c r="D87" s="50"/>
@@ -1840,7 +1837,7 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B88" s="35" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C88" s="52"/>
       <c r="D88" s="53"/>
@@ -1848,7 +1845,7 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B89" s="35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C89" s="52"/>
       <c r="D89" s="53"/>
@@ -1856,7 +1853,7 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B90" s="35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C90" s="52"/>
       <c r="D90" s="53"/>
@@ -1865,7 +1862,7 @@
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" s="24"/>
       <c r="B93" s="58" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C93" s="58"/>
       <c r="D93" s="58"/>
@@ -1902,10 +1899,10 @@
         <v>4</v>
       </c>
       <c r="B96" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C96" s="49" t="s">
         <v>63</v>
-      </c>
-      <c r="C96" s="49" t="s">
-        <v>64</v>
       </c>
       <c r="D96" s="50"/>
       <c r="E96" s="51"/>
@@ -1915,10 +1912,10 @@
         <v>5</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C97" s="52" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D97" s="53"/>
       <c r="E97" s="54"/>
@@ -1938,7 +1935,7 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B100" s="35" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C100" s="6"/>
       <c r="D100" s="7"/>
@@ -1946,7 +1943,7 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B101" s="35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C101" s="55"/>
       <c r="D101" s="56"/>
@@ -1954,7 +1951,7 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B102" s="35" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C102" s="55"/>
       <c r="D102" s="56"/>
@@ -1962,7 +1959,7 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B103" s="35" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C103" s="49"/>
       <c r="D103" s="50"/>
@@ -1970,7 +1967,7 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B104" s="35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C104" s="52"/>
       <c r="D104" s="53"/>
@@ -1989,7 +1986,7 @@
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" s="24"/>
       <c r="B107" s="58" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C107" s="58"/>
       <c r="D107" s="58"/>
@@ -2026,10 +2023,10 @@
         <v>4</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C110" s="49" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D110" s="50"/>
       <c r="E110" s="51"/>
@@ -2039,10 +2036,10 @@
         <v>5</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C111" s="52" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D111" s="53"/>
       <c r="E111" s="54"/>
@@ -2062,7 +2059,7 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B114" s="38" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C114" s="20"/>
       <c r="D114" s="7"/>
@@ -2070,7 +2067,7 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B115" s="38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C115" s="21"/>
       <c r="D115" s="56"/>
@@ -2078,7 +2075,7 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B116" s="38" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C116" s="21"/>
       <c r="D116" s="56"/>
@@ -2086,7 +2083,7 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B117" s="38" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C117" s="22"/>
       <c r="D117" s="50"/>
@@ -2094,7 +2091,7 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B118" s="38" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C118" s="22"/>
       <c r="D118" s="50"/>
@@ -2102,7 +2099,7 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B119" s="38" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C119" s="23"/>
       <c r="D119" s="53"/>
@@ -2110,7 +2107,7 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B120" s="38" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C120" s="23"/>
       <c r="D120" s="53"/>
@@ -2129,7 +2126,7 @@
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" s="24"/>
       <c r="B123" s="58" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C123" s="58"/>
       <c r="D123" s="58"/>
@@ -2166,10 +2163,10 @@
         <v>4</v>
       </c>
       <c r="B126" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C126" s="49" t="s">
         <v>66</v>
-      </c>
-      <c r="C126" s="49" t="s">
-        <v>67</v>
       </c>
       <c r="D126" s="50"/>
       <c r="E126" s="51"/>
@@ -2179,10 +2176,10 @@
         <v>5</v>
       </c>
       <c r="B127" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C127" s="52" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D127" s="53"/>
       <c r="E127" s="54"/>
@@ -2202,7 +2199,7 @@
     </row>
     <row r="130" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B130" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C130" s="20"/>
       <c r="D130" s="7"/>
@@ -2210,7 +2207,7 @@
     </row>
     <row r="131" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B131" s="38" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C131" s="21"/>
       <c r="D131" s="56"/>
@@ -2218,7 +2215,7 @@
     </row>
     <row r="132" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B132" s="38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C132" s="21"/>
       <c r="D132" s="56"/>
@@ -2226,7 +2223,7 @@
     </row>
     <row r="133" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B133" s="38" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C133" s="22"/>
       <c r="D133" s="50"/>
@@ -2234,7 +2231,7 @@
     </row>
     <row r="134" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B134" s="38" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C134" s="22"/>
       <c r="D134" s="50"/>
@@ -2242,7 +2239,7 @@
     </row>
     <row r="135" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B135" s="38" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C135" s="23"/>
       <c r="D135" s="53"/>
@@ -2250,7 +2247,7 @@
     </row>
     <row r="136" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B136" s="38" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C136" s="23"/>
       <c r="D136" s="53"/>
@@ -2258,6 +2255,18 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C46:E46"/>
     <mergeCell ref="C48:E48"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="C41:E41"/>
@@ -2274,18 +2283,6 @@
     <mergeCell ref="B7:E7"/>
     <mergeCell ref="C6:E6"/>
     <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="B43:E43"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C18:E18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>